<commit_message>
Began bundling scripts and styling Created metadata folder
</commit_message>
<xml_diff>
--- a/Magic Item Store Tables.xlsx
+++ b/Magic Item Store Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49cf407edbb941b8/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LiveProjects\StoreFront\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="485" documentId="8_{DB48662D-7A44-41C6-873A-3A1773C71395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C7AB556-1D74-446E-8118-8AE18F141AA1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DC4EDC-8911-4D97-AD14-5967829B0016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{201A3552-3CA4-4243-BFC7-53320D576E04}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="111">
   <si>
     <t>Magic Item Store</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Alchemy Jug</t>
   </si>
   <si>
-    <t>…</t>
-  </si>
-  <si>
     <t>Adventuring Gear</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
     <t>Location</t>
   </si>
   <si>
-    <t>...</t>
-  </si>
-  <si>
     <t>Sunblade</t>
   </si>
   <si>
@@ -165,9 +159,6 @@
     <t>DepartmentName</t>
   </si>
   <si>
-    <t>Item Creation</t>
-  </si>
-  <si>
     <t>Sales</t>
   </si>
   <si>
@@ -226,13 +217,163 @@
   </si>
   <si>
     <t>Statuses</t>
+  </si>
+  <si>
+    <t>MagicItemImage</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>Crudius</t>
+  </si>
+  <si>
+    <t>Crinkle</t>
+  </si>
+  <si>
+    <t>Ianthe</t>
+  </si>
+  <si>
+    <t>Liaphine</t>
+  </si>
+  <si>
+    <t>Portia</t>
+  </si>
+  <si>
+    <t>Florentius</t>
+  </si>
+  <si>
+    <t>Arynthya</t>
+  </si>
+  <si>
+    <t>Glassgleam</t>
+  </si>
+  <si>
+    <t>Goodearth</t>
+  </si>
+  <si>
+    <t>Rhyp</t>
+  </si>
+  <si>
+    <t>Mistwick</t>
+  </si>
+  <si>
+    <t>The Mazarine City</t>
+  </si>
+  <si>
+    <t>This sword hovers in front of you, attacking creatures who come too close and flying out to attack those at range.</t>
+  </si>
+  <si>
+    <t>When you speak this magic sword’s command word, flames erupt from the blade. These flames shed bright light and deal extra fire damage.</t>
+  </si>
+  <si>
+    <t>This staff gives you the power to cast cold damage spells. You also have resistance to cold damage while you hold this staff.</t>
+  </si>
+  <si>
+    <t>This item appears to be a longsword hilt. While grasping the hilt, you can use a bonus action to cause a blade of pure radiance to spring into existence, or make the blade disappear.</t>
+  </si>
+  <si>
+    <t>This sword has a higher chance of lopping off your opponent’s limbs.</t>
+  </si>
+  <si>
+    <t>This ceramic jug appears to be able to hold a gallon of liquid and weighs 12 pounds whether full or empty. Speak the name of one of the following liquids, uncork the jug and that liquid will pour the liquid out, 2 gallons per minute: ale, honey, mayonnaise, vinegar, water, wine.</t>
+  </si>
+  <si>
+    <t>This wooden broom, which weighs 3 pounds, functions like a mundane broom until you stand astride it and speak its command word. It then hovers beneath you and can be ridden in the air.</t>
+  </si>
+  <si>
+    <t>This small sphere of thick glass weighs 1 pound. If you speak its command word, it emanates light.</t>
+  </si>
+  <si>
+    <t>This flat iron rod has a button on one end. You can use an action to press the button, which causes the rod to become magically fixed in place. Until you or another creature uses an action to push the button again, the rod doesn't move, even if it is defying gravity.</t>
+  </si>
+  <si>
+    <t>Sending stones come in pairs, with each smooth stone carved to match the other so the pairing is easily recognized. While touching one stone each, two people can speak to each other over great distances.</t>
+  </si>
+  <si>
+    <t>This bag has an interior space considerably larger than its outside dimensions, roughly 2 feet in diameter at the mouth and 4 feet deep. The bag can hold up to 500 pounds, not exceeding a volume of 64 cubic feet. The bag weighs 15 pounds, regardless of its contents.</t>
+  </si>
+  <si>
+    <t>You gain extra protection while you wear this cloak.</t>
+  </si>
+  <si>
+    <t>These gloves seem to almost meld into your hands when you don them. These help you attempt to catch ranged attacks aimed toward you.</t>
+  </si>
+  <si>
+    <t>While wearing these dark lenses, you can see in the dark out to a range of 60 feet.</t>
+  </si>
+  <si>
+    <t>This necklace has 8 beads hanging from it. You can detach a bead and throw it up to 60 feet away. When it reaches the end of its trajectory, the bead detonates as a fireball.</t>
+  </si>
+  <si>
+    <t>While you wear this pendant, whenever you fall unconscious, you are more easily stabilized. You also heal far faster and more easily.</t>
+  </si>
+  <si>
+    <t>When you fall while wearing this ring, you float to the ground and take no damage from falling.</t>
+  </si>
+  <si>
+    <t>While wearing this ring, you are immune to magic that allows other creatures to read your thoughts or determine whether you are lying. Creatures can telepathically communicate with you only if you allow it.</t>
+  </si>
+  <si>
+    <t>While you wear these light shoes, you can move up, down, and across vertical surfaces and upside down along ceilings, while leaving your hands free.</t>
+  </si>
+  <si>
+    <t>These boots allow you to fly.</t>
+  </si>
+  <si>
+    <t>Dagny</t>
+  </si>
+  <si>
+    <t>Feldspar</t>
+  </si>
+  <si>
+    <t>Elodie</t>
+  </si>
+  <si>
+    <t>Hawthorne</t>
+  </si>
+  <si>
+    <t>Fenwick</t>
+  </si>
+  <si>
+    <t>Stillbrook</t>
+  </si>
+  <si>
+    <t>Gerwyn</t>
+  </si>
+  <si>
+    <t>Errodall</t>
+  </si>
+  <si>
+    <t>Kent</t>
+  </si>
+  <si>
+    <t>Appleby</t>
+  </si>
+  <si>
+    <t>Qualen</t>
+  </si>
+  <si>
+    <t>Oatdust</t>
+  </si>
+  <si>
+    <t>Romhilda</t>
+  </si>
+  <si>
+    <t>Thamior</t>
+  </si>
+  <si>
+    <t>Vonrik</t>
+  </si>
+  <si>
+    <t>Silverfist</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +388,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -269,10 +416,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -587,58 +735,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E62AD9EB-F370-430E-9C60-1E4D0649ECE6}">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.44140625" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -647,22 +792,25 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>59</v>
+        <v>27</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -672,8 +820,8 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
+      <c r="C4" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -687,20 +835,11 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" t="s">
-        <v>30</v>
-      </c>
-      <c r="N4" t="s">
-        <v>31</v>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -708,10 +847,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -725,20 +864,20 @@
       <c r="G5">
         <v>1</v>
       </c>
-      <c r="H5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>27</v>
       </c>
       <c r="L5" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="M5" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="N5" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -746,10 +885,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
+        <v>32</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -763,20 +902,20 @@
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="H6" t="s">
-        <v>5</v>
+      <c r="H6">
+        <v>3</v>
       </c>
       <c r="K6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="M6" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="N6" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -784,10 +923,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="D7">
         <v>3</v>
@@ -801,20 +940,20 @@
       <c r="G7">
         <v>1</v>
       </c>
-      <c r="H7" t="s">
-        <v>5</v>
+      <c r="H7">
+        <v>4</v>
       </c>
       <c r="K7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L7" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="M7" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="N7" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -822,10 +961,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
+        <v>35</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -839,20 +978,20 @@
       <c r="G8">
         <v>1</v>
       </c>
-      <c r="H8" t="s">
-        <v>5</v>
+      <c r="H8">
+        <v>4</v>
       </c>
       <c r="K8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L8" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="M8" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="N8" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -860,10 +999,10 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -877,20 +1016,20 @@
       <c r="G9">
         <v>1</v>
       </c>
-      <c r="H9" t="s">
-        <v>5</v>
+      <c r="H9">
+        <v>1</v>
       </c>
       <c r="K9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L9" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="M9" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="N9" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -898,10 +1037,10 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
+        <v>37</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -915,11 +1054,8 @@
       <c r="G10">
         <v>1</v>
       </c>
-      <c r="H10" t="s">
-        <v>5</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>48</v>
+      <c r="H10">
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -927,10 +1063,10 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
+        <v>34</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -944,11 +1080,8 @@
       <c r="G11">
         <v>1</v>
       </c>
-      <c r="H11" t="s">
-        <v>5</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>59</v>
+      <c r="H11">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -956,10 +1089,10 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -973,14 +1106,8 @@
       <c r="G12">
         <v>1</v>
       </c>
-      <c r="H12" t="s">
-        <v>5</v>
-      </c>
-      <c r="K12" t="s">
-        <v>41</v>
-      </c>
-      <c r="L12" t="s">
-        <v>42</v>
+      <c r="H12">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -988,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1005,14 +1132,8 @@
       <c r="G13">
         <v>1</v>
       </c>
-      <c r="H13" t="s">
-        <v>5</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13" t="s">
-        <v>45</v>
+      <c r="H13">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -1020,10 +1141,10 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1037,14 +1158,8 @@
       <c r="G14">
         <v>1</v>
       </c>
-      <c r="H14" t="s">
-        <v>5</v>
-      </c>
-      <c r="K14">
-        <v>2</v>
-      </c>
-      <c r="L14" t="s">
-        <v>43</v>
+      <c r="H14">
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -1052,10 +1167,10 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
+        <v>33</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1069,14 +1184,8 @@
       <c r="G15">
         <v>1</v>
       </c>
-      <c r="H15" t="s">
-        <v>5</v>
-      </c>
-      <c r="K15">
-        <v>3</v>
-      </c>
-      <c r="L15" t="s">
-        <v>44</v>
+      <c r="H15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -1084,10 +1193,10 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
+        <v>36</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1101,8 +1210,8 @@
       <c r="G16">
         <v>1</v>
       </c>
-      <c r="H16" t="s">
-        <v>5</v>
+      <c r="H16">
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -1110,10 +1219,10 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
+        <v>14</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1127,8 +1236,11 @@
       <c r="G17">
         <v>1</v>
       </c>
-      <c r="H17" t="s">
-        <v>5</v>
+      <c r="H17">
+        <v>4</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -1136,10 +1248,10 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1153,8 +1265,11 @@
       <c r="G18">
         <v>1</v>
       </c>
-      <c r="H18" t="s">
-        <v>5</v>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -1162,10 +1277,10 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -1179,8 +1294,14 @@
       <c r="G19">
         <v>1</v>
       </c>
-      <c r="H19" t="s">
-        <v>5</v>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="K19" t="s">
+        <v>39</v>
+      </c>
+      <c r="L19" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -1188,10 +1309,10 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="D20">
         <v>2</v>
@@ -1200,13 +1321,19 @@
         <v>3</v>
       </c>
       <c r="F20">
-        <v>750</v>
+        <v>850</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
-      <c r="H20" t="s">
-        <v>5</v>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -1214,10 +1341,10 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" t="s">
-        <v>5</v>
+        <v>21</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="D21">
         <v>2</v>
@@ -1231,8 +1358,14 @@
       <c r="G21">
         <v>1</v>
       </c>
-      <c r="H21" t="s">
-        <v>5</v>
+      <c r="H21">
+        <v>3</v>
+      </c>
+      <c r="K21">
+        <v>2</v>
+      </c>
+      <c r="L21" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -1240,10 +1373,10 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5</v>
+        <v>31</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -1257,8 +1390,14 @@
       <c r="G22">
         <v>1</v>
       </c>
-      <c r="H22" t="s">
-        <v>5</v>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="K22">
+        <v>3</v>
+      </c>
+      <c r="L22" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -1266,10 +1405,10 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" t="s">
-        <v>5</v>
+        <v>22</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="D23">
         <v>2</v>
@@ -1283,77 +1422,77 @@
       <c r="G23">
         <v>1</v>
       </c>
-      <c r="H23" t="s">
-        <v>5</v>
+      <c r="H23">
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N26" t="s">
+        <v>58</v>
+      </c>
+      <c r="O26" t="s">
         <v>59</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="N26" t="s">
-        <v>62</v>
-      </c>
-      <c r="O26" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s">
         <v>24</v>
       </c>
-      <c r="C27" t="s">
+      <c r="E27" t="s">
         <v>25</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>26</v>
       </c>
-      <c r="F27" t="s">
-        <v>27</v>
-      </c>
       <c r="H27" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I27" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K27" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L27" t="s">
+        <v>28</v>
+      </c>
+      <c r="M27" t="s">
         <v>29</v>
       </c>
-      <c r="M27" t="s">
-        <v>30</v>
-      </c>
       <c r="N27" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="O27" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
@@ -1361,22 +1500,31 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K28">
         <v>1</v>
+      </c>
+      <c r="L28" t="s">
+        <v>95</v>
+      </c>
+      <c r="M28" t="s">
+        <v>96</v>
+      </c>
+      <c r="N28">
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -1384,22 +1532,34 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E29">
         <v>2</v>
       </c>
       <c r="F29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H29">
         <v>2</v>
       </c>
       <c r="I29" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K29">
         <v>2</v>
+      </c>
+      <c r="L29" t="s">
+        <v>97</v>
+      </c>
+      <c r="M29" t="s">
+        <v>98</v>
+      </c>
+      <c r="N29">
+        <v>2</v>
+      </c>
+      <c r="O29" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -1407,22 +1567,34 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E30">
         <v>3</v>
       </c>
       <c r="F30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H30">
         <v>3</v>
       </c>
       <c r="I30" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K30">
         <v>3</v>
+      </c>
+      <c r="L30" t="s">
+        <v>99</v>
+      </c>
+      <c r="M30" t="s">
+        <v>100</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+      <c r="O30" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
@@ -1430,13 +1602,93 @@
         <v>4</v>
       </c>
       <c r="F31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H31">
         <v>4</v>
       </c>
       <c r="I31" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="K31">
+        <v>4</v>
+      </c>
+      <c r="L31" t="s">
+        <v>101</v>
+      </c>
+      <c r="M31" t="s">
+        <v>102</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K32">
+        <v>5</v>
+      </c>
+      <c r="L32" t="s">
+        <v>103</v>
+      </c>
+      <c r="M32" t="s">
+        <v>104</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+      <c r="O32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="11:15" x14ac:dyDescent="0.3">
+      <c r="K33">
+        <v>6</v>
+      </c>
+      <c r="L33" t="s">
+        <v>105</v>
+      </c>
+      <c r="M33" t="s">
+        <v>106</v>
+      </c>
+      <c r="N33">
+        <v>1</v>
+      </c>
+      <c r="O33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="11:15" x14ac:dyDescent="0.3">
+      <c r="K34">
+        <v>7</v>
+      </c>
+      <c r="L34" t="s">
+        <v>107</v>
+      </c>
+      <c r="M34" t="s">
+        <v>108</v>
+      </c>
+      <c r="N34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="11:15" x14ac:dyDescent="0.3">
+      <c r="K35">
+        <v>8</v>
+      </c>
+      <c r="L35" t="s">
+        <v>109</v>
+      </c>
+      <c r="M35" t="s">
+        <v>110</v>
+      </c>
+      <c r="N35">
+        <v>2</v>
+      </c>
+      <c r="O35" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>